<commit_message>
feat: Agregar nuevo modo de actualizar plantilla
</commit_message>
<xml_diff>
--- a/data/segmentacion_demo.xlsx
+++ b/data/segmentacion_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F669BD92-E21B-A74F-9E2B-201F82EF7274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF172B6-AF07-C24D-B66F-2368EC720894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30260" yWindow="600" windowWidth="38380" windowHeight="21000" activeTab="1" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Aperturas_Siniestros" sheetId="13" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="101">
   <si>
     <t>Amparo_Desc</t>
   </si>
@@ -336,6 +336,15 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>Mensual</t>
+  </si>
+  <si>
+    <t>Semestral</t>
+  </si>
+  <si>
+    <t>Anual</t>
   </si>
 </sst>
 </file>
@@ -859,8 +868,8 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -953,7 +962,7 @@
         <v>96</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -974,7 +983,7 @@
         <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -995,7 +1004,7 @@
         <v>96</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1016,7 +1025,7 @@
         <v>97</v>
       </c>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1037,7 +1046,7 @@
         <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1058,7 +1067,7 @@
         <v>97</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1078,7 +1087,7 @@
   </sheetPr>
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2338,26 +2347,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e625656c-bba3-4077-8eff-14104607af5a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="92acd330-8342-45fc-be4b-65850f6282f9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CF4D88A847C084DB84844F39084E439" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="451e82d02e108cc447a9cc14d7f86033">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92acd330-8342-45fc-be4b-65850f6282f9" xmlns:ns3="e625656c-bba3-4077-8eff-14104607af5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2eae878ca301ee5618ce7adadc34258d" ns2:_="" ns3:_="">
     <xsd:import namespace="92acd330-8342-45fc-be4b-65850f6282f9"/>
@@ -2558,6 +2547,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e625656c-bba3-4077-8eff-14104607af5a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="92acd330-8342-45fc-be4b-65850f6282f9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <Application xmlns="http://www.sap.com/cof/excel/application">
   <Version>2</Version>
@@ -2566,9 +2575,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62D4AD73-2F3B-41AE-8958-0F3FAF115B0E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="92acd330-8342-45fc-be4b-65850f6282f9"/>
+    <ds:schemaRef ds:uri="e625656c-bba3-4077-8eff-14104607af5a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2594,20 +2614,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62D4AD73-2F3B-41AE-8958-0F3FAF115B0E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="92acd330-8342-45fc-be4b-65850f6282f9"/>
-    <ds:schemaRef ds:uri="e625656c-bba3-4077-8eff-14104607af5a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: Agregar metodologias de indexacion de severidad
</commit_message>
<xml_diff>
--- a/data/segmentacion_demo.xlsx
+++ b/data/segmentacion_demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF172B6-AF07-C24D-B66F-2368EC720894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFA207D-E1E3-4546-A238-D2D256D35356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="108">
   <si>
     <t>Amparo_Desc</t>
   </si>
@@ -345,6 +345,27 @@
   </si>
   <si>
     <t>Anual</t>
+  </si>
+  <si>
+    <t>tipo_indexacion_severidad</t>
+  </si>
+  <si>
+    <t>medida_indexacion_severidad</t>
+  </si>
+  <si>
+    <t>Ninguna</t>
+  </si>
+  <si>
+    <t>Por fecha de ocurrencia</t>
+  </si>
+  <si>
+    <t>Por fecha de movimiento</t>
+  </si>
+  <si>
+    <t>IPC</t>
+  </si>
+  <si>
+    <t>SMMLV</t>
   </si>
 </sst>
 </file>
@@ -866,10 +887,10 @@
   <sheetPr codeName="Hoja5">
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,9 +901,11 @@
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
@@ -901,8 +924,14 @@
       <c r="F1" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>+B2&amp;"_"&amp;C2&amp;"_"&amp;D2&amp;"_"&amp;E2</f>
         <v>01_001_A_D</v>
@@ -922,8 +951,14 @@
       <c r="F2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A9" si="0">+B3&amp;"_"&amp;C3&amp;"_"&amp;D3&amp;"_"&amp;E3</f>
         <v>01_001_A_E</v>
@@ -943,8 +978,14 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>01_001_B_D</v>
@@ -964,8 +1005,14 @@
       <c r="F4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>01_001_B_E</v>
@@ -985,8 +1032,14 @@
       <c r="F5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>01_002_A_D</v>
@@ -1006,8 +1059,14 @@
       <c r="F6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>01_002_A_E</v>
@@ -1027,8 +1086,14 @@
       <c r="F7" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>01_002_B_D</v>
@@ -1048,8 +1113,14 @@
       <c r="F8" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>01_002_B_E</v>
@@ -1069,11 +1140,20 @@
       <c r="F9" t="s">
         <v>100</v>
       </c>
+      <c r="G9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{22BE6280-917F-9E46-82F3-4F72A7A28E95}">
       <formula1>"Mensual,Trimestral,Semestral,Anual"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9 H8:H9" xr:uid="{78080211-09A0-9C48-99A5-2543A10E981E}">
+      <formula1>"Ninguna,Por fecha de ocurrencia,Por fecha de movimiento"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2347,6 +2427,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e625656c-bba3-4077-8eff-14104607af5a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="92acd330-8342-45fc-be4b-65850f6282f9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CF4D88A847C084DB84844F39084E439" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="451e82d02e108cc447a9cc14d7f86033">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92acd330-8342-45fc-be4b-65850f6282f9" xmlns:ns3="e625656c-bba3-4077-8eff-14104607af5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2eae878ca301ee5618ce7adadc34258d" ns2:_="" ns3:_="">
     <xsd:import namespace="92acd330-8342-45fc-be4b-65850f6282f9"/>
@@ -2547,18 +2638,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e625656c-bba3-4077-8eff-14104607af5a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="92acd330-8342-45fc-be4b-65850f6282f9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2567,33 +2654,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62D4AD73-2F3B-41AE-8958-0F3FAF115B0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="92acd330-8342-45fc-be4b-65850f6282f9"/>
-    <ds:schemaRef ds:uri="e625656c-bba3-4077-8eff-14104607af5a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2613,18 +2674,37 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62D4AD73-2F3B-41AE-8958-0F3FAF115B0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="92acd330-8342-45fc-be4b-65850f6282f9"/>
+    <ds:schemaRef ds:uri="e625656c-bba3-4077-8eff-14104607af5a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor: Eliminar columna apertura_reservas de archivo segmentacion
</commit_message>
<xml_diff>
--- a/data/segmentacion_demo.xlsx
+++ b/data/segmentacion_demo.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324B874B-E6C0-FA40-A439-E875AD8F103B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aperturas_Siniestros" sheetId="1" r:id="rId1"/>
     <sheet name="Aperturas_Primas" sheetId="2" r:id="rId2"/>
     <sheet name="Aperturas_Expuestos" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="32">
-  <si>
-    <t>apertura_reservas</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="23">
   <si>
     <t>codigo_op</t>
   </si>
@@ -42,9 +45,6 @@
     <t>medida_indexacion_severidad</t>
   </si>
   <si>
-    <t>01_001_A_D</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -63,27 +63,15 @@
     <t>Ninguna</t>
   </si>
   <si>
-    <t>01_001_A_E</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
-    <t>01_001_B_D</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
     <t>Mensual</t>
   </si>
   <si>
-    <t>01_001_B_E</t>
-  </si>
-  <si>
-    <t>01_002_A_D</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -96,29 +84,20 @@
     <t>SMMLV</t>
   </si>
   <si>
-    <t>01_002_A_E</t>
-  </si>
-  <si>
     <t>Por fecha de movimiento</t>
   </si>
   <si>
     <t>IPC</t>
   </si>
   <si>
-    <t>01_002_B_D</t>
-  </si>
-  <si>
     <t>Anual</t>
-  </si>
-  <si>
-    <t>01_002_B_E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,60 +135,65 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf/>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:H9" totalsRowShown="0">
-  <autoFilter ref="A1:H9"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="apertura_reservas" dataDxfId="0"/>
-    <tableColumn id="2" name="codigo_op" dataDxfId="0"/>
-    <tableColumn id="3" name="codigo_ramo_op" dataDxfId="0"/>
-    <tableColumn id="4" name="apertura_1" dataDxfId="0"/>
-    <tableColumn id="5" name="apertura_2" dataDxfId="0"/>
-    <tableColumn id="6" name="periodicidad_ocurrencia" dataDxfId="0"/>
-    <tableColumn id="7" name="tipo_indexacion_severidad" dataDxfId="0"/>
-    <tableColumn id="8" name="medida_indexacion_severidad" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Frame0" displayName="Frame0" ref="A1:G9" totalsRowShown="0">
+  <autoFilter ref="A1:G9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="codigo_op"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="codigo_ramo_op"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="apertura_1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="apertura_2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="periodicidad_ocurrencia"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="tipo_indexacion_severidad"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="medida_indexacion_severidad"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Frame1" displayName="Frame1" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Frame1" displayName="Frame1" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="codigo_op" dataDxfId="0"/>
-    <tableColumn id="2" name="codigo_ramo_op" dataDxfId="0"/>
-    <tableColumn id="3" name="apertura_1" dataDxfId="0"/>
-    <tableColumn id="4" name="apertura_2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="codigo_op"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="codigo_ramo_op"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="apertura_1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="apertura_2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Frame2" displayName="Frame2" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Frame2" displayName="Frame2" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="codigo_op" dataDxfId="0"/>
-    <tableColumn id="2" name="codigo_ramo_op" dataDxfId="0"/>
-    <tableColumn id="3" name="apertura_1" dataDxfId="0"/>
-    <tableColumn id="4" name="apertura_2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="codigo_op"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="codigo_ramo_op"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="apertura_1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="apertura_2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -247,7 +231,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -281,6 +265,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -315,9 +300,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -490,14 +476,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,216 +507,189 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -740,137 +701,137 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -882,137 +843,137 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>